<commit_message>
EBEGU-2006: Column Kinder renamed to Kind1 to KindN
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Massenversand.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Massenversand.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\G$\hefr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denise\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C886365A-A591-4E5E-8D6F-C29896856D2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16D46E4-9B09-41E7-93BD-7EEFCC6169C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="20565" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10590" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="77">
   <si>
     <t>Parameter</t>
   </si>
@@ -161,9 +156,6 @@
     <t>Dubletten</t>
   </si>
   <si>
-    <t>Kinder</t>
-  </si>
-  <si>
     <t>Kita</t>
   </si>
   <si>
@@ -234,6 +226,36 @@
   </si>
   <si>
     <t>Kontaktdaten für Serienbriefe</t>
+  </si>
+  <si>
+    <t>Kind 1</t>
+  </si>
+  <si>
+    <t>Kind 2</t>
+  </si>
+  <si>
+    <t>Kind 3</t>
+  </si>
+  <si>
+    <t>Kind 4</t>
+  </si>
+  <si>
+    <t>Kind 5</t>
+  </si>
+  <si>
+    <t>Kind 6</t>
+  </si>
+  <si>
+    <t>Kind 7</t>
+  </si>
+  <si>
+    <t>Kind 8</t>
+  </si>
+  <si>
+    <t>Kind 9</t>
+  </si>
+  <si>
+    <t>Kind 10</t>
   </si>
 </sst>
 </file>
@@ -435,8 +457,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -457,13 +484,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -875,8 +897,8 @@
   </sheetPr>
   <dimension ref="A1:DV16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,7 +990,7 @@
   <sheetData>
     <row r="1" spans="1:126" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1058,10 +1080,10 @@
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1069,1005 +1091,1005 @@
     <row r="12" spans="1:126" x14ac:dyDescent="0.25">
       <c r="C12"/>
       <c r="L12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="R12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="V12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="W12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Z12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AA12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AB12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AC12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AD12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AE12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AF12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AH12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AI12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AJ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AK12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AL12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AM12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AN12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AO12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AP12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AQ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AR12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AS12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AT12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AU12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AV12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AW12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AX12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AY12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AZ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BA12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BB12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BC12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BD12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BE12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BF12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BG12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BH12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BI12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BJ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BK12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BL12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BM12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BN12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BO12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BP12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BQ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BR12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BS12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BT12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BU12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BV12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BW12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BX12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BY12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BZ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CA12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CB12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CC12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CD12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CE12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CF12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CG12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CH12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CI12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CJ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CK12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CL12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CM12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CN12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CO12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CP12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CQ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CR12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CS12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CT12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CU12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CV12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CW12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CX12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CY12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CZ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DA12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DB12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DC12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DD12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DE12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DF12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DG12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DH12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DI12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DJ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DK12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DL12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DM12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DN12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DO12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DP12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="DQ12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:126" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="25" t="s">
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="L13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
-      <c r="AG13" s="18"/>
-      <c r="AH13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI13" s="18"/>
-      <c r="AJ13" s="18"/>
-      <c r="AK13" s="18"/>
-      <c r="AL13" s="18"/>
-      <c r="AM13" s="18"/>
-      <c r="AN13" s="18"/>
-      <c r="AO13" s="18"/>
-      <c r="AP13" s="18"/>
-      <c r="AQ13" s="18"/>
-      <c r="AR13" s="18"/>
-      <c r="AS13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT13" s="18"/>
-      <c r="AU13" s="18"/>
-      <c r="AV13" s="18"/>
-      <c r="AW13" s="18"/>
-      <c r="AX13" s="18"/>
-      <c r="AY13" s="18"/>
-      <c r="AZ13" s="18"/>
-      <c r="BA13" s="18"/>
-      <c r="BB13" s="18"/>
-      <c r="BC13" s="18"/>
-      <c r="BD13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="BE13" s="18"/>
-      <c r="BF13" s="18"/>
-      <c r="BG13" s="18"/>
-      <c r="BH13" s="18"/>
-      <c r="BI13" s="18"/>
-      <c r="BJ13" s="18"/>
-      <c r="BK13" s="18"/>
-      <c r="BL13" s="18"/>
-      <c r="BM13" s="18"/>
-      <c r="BN13" s="18"/>
-      <c r="BO13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="BP13" s="18"/>
-      <c r="BQ13" s="18"/>
-      <c r="BR13" s="18"/>
-      <c r="BS13" s="18"/>
-      <c r="BT13" s="18"/>
-      <c r="BU13" s="18"/>
-      <c r="BV13" s="18"/>
-      <c r="BW13" s="18"/>
-      <c r="BX13" s="18"/>
-      <c r="BY13" s="18"/>
-      <c r="BZ13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="CA13" s="18"/>
-      <c r="CB13" s="18"/>
-      <c r="CC13" s="18"/>
-      <c r="CD13" s="18"/>
-      <c r="CE13" s="18"/>
-      <c r="CF13" s="18"/>
-      <c r="CG13" s="18"/>
-      <c r="CH13" s="18"/>
-      <c r="CI13" s="18"/>
-      <c r="CJ13" s="18"/>
-      <c r="CK13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="CL13" s="18"/>
-      <c r="CM13" s="18"/>
-      <c r="CN13" s="18"/>
-      <c r="CO13" s="18"/>
-      <c r="CP13" s="18"/>
-      <c r="CQ13" s="18"/>
-      <c r="CR13" s="18"/>
-      <c r="CS13" s="18"/>
-      <c r="CT13" s="18"/>
-      <c r="CU13" s="18"/>
-      <c r="CV13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="CW13" s="18"/>
-      <c r="CX13" s="18"/>
-      <c r="CY13" s="18"/>
-      <c r="CZ13" s="18"/>
-      <c r="DA13" s="18"/>
-      <c r="DB13" s="18"/>
-      <c r="DC13" s="18"/>
-      <c r="DD13" s="18"/>
-      <c r="DE13" s="18"/>
-      <c r="DF13" s="18"/>
-      <c r="DG13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="DH13" s="18"/>
-      <c r="DI13" s="18"/>
-      <c r="DJ13" s="18"/>
-      <c r="DK13" s="18"/>
-      <c r="DL13" s="18"/>
-      <c r="DM13" s="18"/>
-      <c r="DN13" s="18"/>
-      <c r="DO13" s="18"/>
-      <c r="DP13" s="18"/>
-      <c r="DQ13" s="18"/>
-      <c r="DR13" s="22" t="s">
+      <c r="L13" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AD13" s="28"/>
+      <c r="AE13" s="28"/>
+      <c r="AF13" s="28"/>
+      <c r="AG13" s="28"/>
+      <c r="AH13" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI13" s="28"/>
+      <c r="AJ13" s="28"/>
+      <c r="AK13" s="28"/>
+      <c r="AL13" s="28"/>
+      <c r="AM13" s="28"/>
+      <c r="AN13" s="28"/>
+      <c r="AO13" s="28"/>
+      <c r="AP13" s="28"/>
+      <c r="AQ13" s="28"/>
+      <c r="AR13" s="28"/>
+      <c r="AS13" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT13" s="28"/>
+      <c r="AU13" s="28"/>
+      <c r="AV13" s="28"/>
+      <c r="AW13" s="28"/>
+      <c r="AX13" s="28"/>
+      <c r="AY13" s="28"/>
+      <c r="AZ13" s="28"/>
+      <c r="BA13" s="28"/>
+      <c r="BB13" s="28"/>
+      <c r="BC13" s="28"/>
+      <c r="BD13" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="BE13" s="28"/>
+      <c r="BF13" s="28"/>
+      <c r="BG13" s="28"/>
+      <c r="BH13" s="28"/>
+      <c r="BI13" s="28"/>
+      <c r="BJ13" s="28"/>
+      <c r="BK13" s="28"/>
+      <c r="BL13" s="28"/>
+      <c r="BM13" s="28"/>
+      <c r="BN13" s="28"/>
+      <c r="BO13" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="BP13" s="28"/>
+      <c r="BQ13" s="28"/>
+      <c r="BR13" s="28"/>
+      <c r="BS13" s="28"/>
+      <c r="BT13" s="28"/>
+      <c r="BU13" s="28"/>
+      <c r="BV13" s="28"/>
+      <c r="BW13" s="28"/>
+      <c r="BX13" s="28"/>
+      <c r="BY13" s="28"/>
+      <c r="BZ13" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="CA13" s="28"/>
+      <c r="CB13" s="28"/>
+      <c r="CC13" s="28"/>
+      <c r="CD13" s="28"/>
+      <c r="CE13" s="28"/>
+      <c r="CF13" s="28"/>
+      <c r="CG13" s="28"/>
+      <c r="CH13" s="28"/>
+      <c r="CI13" s="28"/>
+      <c r="CJ13" s="28"/>
+      <c r="CK13" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="CL13" s="28"/>
+      <c r="CM13" s="28"/>
+      <c r="CN13" s="28"/>
+      <c r="CO13" s="28"/>
+      <c r="CP13" s="28"/>
+      <c r="CQ13" s="28"/>
+      <c r="CR13" s="28"/>
+      <c r="CS13" s="28"/>
+      <c r="CT13" s="28"/>
+      <c r="CU13" s="28"/>
+      <c r="CV13" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="CW13" s="28"/>
+      <c r="CX13" s="28"/>
+      <c r="CY13" s="28"/>
+      <c r="CZ13" s="28"/>
+      <c r="DA13" s="28"/>
+      <c r="DB13" s="28"/>
+      <c r="DC13" s="28"/>
+      <c r="DD13" s="28"/>
+      <c r="DE13" s="28"/>
+      <c r="DF13" s="28"/>
+      <c r="DG13" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="DH13" s="28"/>
+      <c r="DI13" s="28"/>
+      <c r="DJ13" s="28"/>
+      <c r="DK13" s="28"/>
+      <c r="DL13" s="28"/>
+      <c r="DM13" s="28"/>
+      <c r="DN13" s="28"/>
+      <c r="DO13" s="28"/>
+      <c r="DP13" s="28"/>
+      <c r="DQ13" s="28"/>
+      <c r="DR13" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="DS13" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="DS13" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="DT13" s="22" t="s">
-        <v>52</v>
+      <c r="DT13" s="25" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:126" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="18" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="18" t="s">
+      <c r="K14" s="21"/>
+      <c r="L14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="M14" s="18" t="s">
+      <c r="M14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="N14" s="18" t="s">
+      <c r="N14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="18" t="s">
+      <c r="O14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="P14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="18" t="s">
+      <c r="P14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="X14" s="18" t="s">
+      <c r="X14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="Y14" s="18" t="s">
+      <c r="Y14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="Z14" s="18" t="s">
+      <c r="Z14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="AA14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB14" s="20"/>
-      <c r="AC14" s="20"/>
-      <c r="AD14" s="20"/>
-      <c r="AE14" s="20"/>
-      <c r="AF14" s="20"/>
-      <c r="AG14" s="21"/>
-      <c r="AH14" s="18" t="s">
+      <c r="AA14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB14" s="23"/>
+      <c r="AC14" s="23"/>
+      <c r="AD14" s="23"/>
+      <c r="AE14" s="23"/>
+      <c r="AF14" s="23"/>
+      <c r="AG14" s="24"/>
+      <c r="AH14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="AI14" s="18" t="s">
+      <c r="AI14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AJ14" s="18" t="s">
+      <c r="AJ14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AK14" s="18" t="s">
+      <c r="AK14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="AL14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM14" s="20"/>
-      <c r="AN14" s="20"/>
-      <c r="AO14" s="20"/>
-      <c r="AP14" s="20"/>
-      <c r="AQ14" s="20"/>
-      <c r="AR14" s="21"/>
-      <c r="AS14" s="18" t="s">
+      <c r="AL14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM14" s="23"/>
+      <c r="AN14" s="23"/>
+      <c r="AO14" s="23"/>
+      <c r="AP14" s="23"/>
+      <c r="AQ14" s="23"/>
+      <c r="AR14" s="24"/>
+      <c r="AS14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="AT14" s="18" t="s">
+      <c r="AT14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AU14" s="18" t="s">
+      <c r="AU14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AV14" s="18" t="s">
+      <c r="AV14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="AW14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="AX14" s="20"/>
-      <c r="AY14" s="20"/>
-      <c r="AZ14" s="20"/>
-      <c r="BA14" s="20"/>
-      <c r="BB14" s="20"/>
-      <c r="BC14" s="21"/>
-      <c r="BD14" s="18" t="s">
+      <c r="AW14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX14" s="23"/>
+      <c r="AY14" s="23"/>
+      <c r="AZ14" s="23"/>
+      <c r="BA14" s="23"/>
+      <c r="BB14" s="23"/>
+      <c r="BC14" s="24"/>
+      <c r="BD14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="BE14" s="18" t="s">
+      <c r="BE14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="BF14" s="18" t="s">
+      <c r="BF14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="BG14" s="18" t="s">
+      <c r="BG14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="BH14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="BI14" s="20"/>
-      <c r="BJ14" s="20"/>
-      <c r="BK14" s="20"/>
-      <c r="BL14" s="20"/>
-      <c r="BM14" s="20"/>
-      <c r="BN14" s="21"/>
-      <c r="BO14" s="18" t="s">
+      <c r="BH14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="BI14" s="23"/>
+      <c r="BJ14" s="23"/>
+      <c r="BK14" s="23"/>
+      <c r="BL14" s="23"/>
+      <c r="BM14" s="23"/>
+      <c r="BN14" s="24"/>
+      <c r="BO14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="BP14" s="18" t="s">
+      <c r="BP14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="BQ14" s="18" t="s">
+      <c r="BQ14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="BR14" s="18" t="s">
+      <c r="BR14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="BS14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="BT14" s="20"/>
-      <c r="BU14" s="20"/>
-      <c r="BV14" s="20"/>
-      <c r="BW14" s="20"/>
-      <c r="BX14" s="20"/>
-      <c r="BY14" s="21"/>
-      <c r="BZ14" s="18" t="s">
+      <c r="BS14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="BT14" s="23"/>
+      <c r="BU14" s="23"/>
+      <c r="BV14" s="23"/>
+      <c r="BW14" s="23"/>
+      <c r="BX14" s="23"/>
+      <c r="BY14" s="24"/>
+      <c r="BZ14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="CA14" s="18" t="s">
+      <c r="CA14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="CB14" s="18" t="s">
+      <c r="CB14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="CC14" s="18" t="s">
+      <c r="CC14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="CD14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="CE14" s="20"/>
-      <c r="CF14" s="20"/>
-      <c r="CG14" s="20"/>
-      <c r="CH14" s="20"/>
-      <c r="CI14" s="20"/>
-      <c r="CJ14" s="21"/>
-      <c r="CK14" s="18" t="s">
+      <c r="CD14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="CE14" s="23"/>
+      <c r="CF14" s="23"/>
+      <c r="CG14" s="23"/>
+      <c r="CH14" s="23"/>
+      <c r="CI14" s="23"/>
+      <c r="CJ14" s="24"/>
+      <c r="CK14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="CL14" s="18" t="s">
+      <c r="CL14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="CM14" s="18" t="s">
+      <c r="CM14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="CN14" s="18" t="s">
+      <c r="CN14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="CO14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="CP14" s="20"/>
-      <c r="CQ14" s="20"/>
-      <c r="CR14" s="20"/>
-      <c r="CS14" s="20"/>
-      <c r="CT14" s="20"/>
-      <c r="CU14" s="21"/>
-      <c r="CV14" s="18" t="s">
+      <c r="CO14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="CP14" s="23"/>
+      <c r="CQ14" s="23"/>
+      <c r="CR14" s="23"/>
+      <c r="CS14" s="23"/>
+      <c r="CT14" s="23"/>
+      <c r="CU14" s="24"/>
+      <c r="CV14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="CW14" s="18" t="s">
+      <c r="CW14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="CX14" s="18" t="s">
+      <c r="CX14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="CY14" s="18" t="s">
+      <c r="CY14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="CZ14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="DA14" s="20"/>
-      <c r="DB14" s="20"/>
-      <c r="DC14" s="20"/>
-      <c r="DD14" s="20"/>
-      <c r="DE14" s="20"/>
-      <c r="DF14" s="21"/>
-      <c r="DG14" s="18" t="s">
+      <c r="CZ14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="DA14" s="23"/>
+      <c r="DB14" s="23"/>
+      <c r="DC14" s="23"/>
+      <c r="DD14" s="23"/>
+      <c r="DE14" s="23"/>
+      <c r="DF14" s="24"/>
+      <c r="DG14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="DH14" s="18" t="s">
+      <c r="DH14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="DI14" s="18" t="s">
+      <c r="DI14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="DJ14" s="18" t="s">
+      <c r="DJ14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="DK14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="DL14" s="20"/>
-      <c r="DM14" s="20"/>
-      <c r="DN14" s="20"/>
-      <c r="DO14" s="20"/>
-      <c r="DP14" s="20"/>
-      <c r="DQ14" s="21"/>
-      <c r="DR14" s="23"/>
-      <c r="DS14" s="23"/>
-      <c r="DT14" s="23"/>
+      <c r="DK14" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="DL14" s="23"/>
+      <c r="DM14" s="23"/>
+      <c r="DN14" s="23"/>
+      <c r="DO14" s="23"/>
+      <c r="DP14" s="23"/>
+      <c r="DQ14" s="24"/>
+      <c r="DR14" s="26"/>
+      <c r="DS14" s="26"/>
+      <c r="DT14" s="26"/>
     </row>
     <row r="15" spans="1:126" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
       <c r="P15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q15" s="12" t="s">
+      <c r="R15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="R15" s="12" t="s">
+      <c r="S15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="S15" s="12" t="s">
+      <c r="T15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="T15" s="12" t="s">
+      <c r="U15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="U15" s="12" t="s">
+      <c r="V15" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="V15" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="28"/>
       <c r="AA15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AB15" s="12" t="s">
+      <c r="AC15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AC15" s="12" t="s">
+      <c r="AD15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AD15" s="12" t="s">
+      <c r="AE15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AE15" s="12" t="s">
+      <c r="AF15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AF15" s="12" t="s">
+      <c r="AG15" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AG15" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH15" s="18"/>
-      <c r="AI15" s="18"/>
-      <c r="AJ15" s="18"/>
-      <c r="AK15" s="18"/>
+      <c r="AH15" s="28"/>
+      <c r="AI15" s="28"/>
+      <c r="AJ15" s="28"/>
+      <c r="AK15" s="28"/>
       <c r="AL15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AM15" s="12" t="s">
+      <c r="AN15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AN15" s="12" t="s">
+      <c r="AO15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AO15" s="12" t="s">
+      <c r="AP15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AP15" s="12" t="s">
+      <c r="AQ15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AQ15" s="12" t="s">
+      <c r="AR15" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AR15" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS15" s="18"/>
-      <c r="AT15" s="18"/>
-      <c r="AU15" s="18"/>
-      <c r="AV15" s="18"/>
+      <c r="AS15" s="28"/>
+      <c r="AT15" s="28"/>
+      <c r="AU15" s="28"/>
+      <c r="AV15" s="28"/>
       <c r="AW15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AX15" s="14" t="s">
+      <c r="AY15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AY15" s="14" t="s">
+      <c r="AZ15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AZ15" s="14" t="s">
+      <c r="BA15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="BA15" s="14" t="s">
+      <c r="BB15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="BB15" s="14" t="s">
+      <c r="BC15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="BC15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD15" s="18"/>
-      <c r="BE15" s="18"/>
-      <c r="BF15" s="18"/>
-      <c r="BG15" s="18"/>
+      <c r="BD15" s="28"/>
+      <c r="BE15" s="28"/>
+      <c r="BF15" s="28"/>
+      <c r="BG15" s="28"/>
       <c r="BH15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="BI15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="BI15" s="14" t="s">
+      <c r="BJ15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="BJ15" s="14" t="s">
+      <c r="BK15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="BK15" s="14" t="s">
+      <c r="BL15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="BL15" s="14" t="s">
+      <c r="BM15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="BM15" s="14" t="s">
+      <c r="BN15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="BN15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="BO15" s="18"/>
-      <c r="BP15" s="18"/>
-      <c r="BQ15" s="18"/>
-      <c r="BR15" s="18"/>
+      <c r="BO15" s="28"/>
+      <c r="BP15" s="28"/>
+      <c r="BQ15" s="28"/>
+      <c r="BR15" s="28"/>
       <c r="BS15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="BT15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="BT15" s="14" t="s">
+      <c r="BU15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="BU15" s="14" t="s">
+      <c r="BV15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="BV15" s="14" t="s">
+      <c r="BW15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="BW15" s="14" t="s">
+      <c r="BX15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="BX15" s="14" t="s">
+      <c r="BY15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="BY15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="BZ15" s="18"/>
-      <c r="CA15" s="18"/>
-      <c r="CB15" s="18"/>
-      <c r="CC15" s="18"/>
+      <c r="BZ15" s="28"/>
+      <c r="CA15" s="28"/>
+      <c r="CB15" s="28"/>
+      <c r="CC15" s="28"/>
       <c r="CD15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="CE15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="CE15" s="14" t="s">
+      <c r="CF15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="CF15" s="14" t="s">
+      <c r="CG15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="CG15" s="14" t="s">
+      <c r="CH15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="CH15" s="14" t="s">
+      <c r="CI15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="CI15" s="14" t="s">
+      <c r="CJ15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="CJ15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="CK15" s="18"/>
-      <c r="CL15" s="18"/>
-      <c r="CM15" s="18"/>
-      <c r="CN15" s="18"/>
+      <c r="CK15" s="28"/>
+      <c r="CL15" s="28"/>
+      <c r="CM15" s="28"/>
+      <c r="CN15" s="28"/>
       <c r="CO15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="CP15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="CP15" s="14" t="s">
+      <c r="CQ15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="CQ15" s="14" t="s">
+      <c r="CR15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="CR15" s="14" t="s">
+      <c r="CS15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="CS15" s="14" t="s">
+      <c r="CT15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="CT15" s="14" t="s">
+      <c r="CU15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="CU15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="CV15" s="18"/>
-      <c r="CW15" s="18"/>
-      <c r="CX15" s="18"/>
-      <c r="CY15" s="18"/>
+      <c r="CV15" s="28"/>
+      <c r="CW15" s="28"/>
+      <c r="CX15" s="28"/>
+      <c r="CY15" s="28"/>
       <c r="CZ15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="DA15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="DA15" s="14" t="s">
+      <c r="DB15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="DB15" s="14" t="s">
+      <c r="DC15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="DC15" s="14" t="s">
+      <c r="DD15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="DD15" s="14" t="s">
+      <c r="DE15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="DE15" s="14" t="s">
+      <c r="DF15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="DF15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="DG15" s="18"/>
-      <c r="DH15" s="18"/>
-      <c r="DI15" s="18"/>
-      <c r="DJ15" s="18"/>
+      <c r="DG15" s="28"/>
+      <c r="DH15" s="28"/>
+      <c r="DI15" s="28"/>
+      <c r="DJ15" s="28"/>
       <c r="DK15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="DL15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="DL15" s="14" t="s">
+      <c r="DM15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="DM15" s="14" t="s">
+      <c r="DN15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="DN15" s="14" t="s">
+      <c r="DO15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="DO15" s="14" t="s">
+      <c r="DP15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="DP15" s="14" t="s">
+      <c r="DQ15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="DQ15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="DR15" s="24"/>
-      <c r="DS15" s="24"/>
-      <c r="DT15" s="24"/>
+      <c r="DR15" s="27"/>
+      <c r="DS15" s="27"/>
+      <c r="DT15" s="27"/>
     </row>
     <row r="16" spans="1:126" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
@@ -2100,7 +2122,7 @@
       <c r="J16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="K16" s="18" t="s">
         <v>41</v>
       </c>
       <c r="L16" s="11" t="s">
@@ -2113,28 +2135,28 @@
         <v>18</v>
       </c>
       <c r="O16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="P16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="P16" s="11" t="s">
+      <c r="Q16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="R16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="S16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="S16" s="11" t="s">
+      <c r="T16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="11" t="s">
+      <c r="U16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="U16" s="11" t="s">
+      <c r="V16" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="V16" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="W16" s="11" t="s">
         <v>16</v>
@@ -2146,28 +2168,28 @@
         <v>18</v>
       </c>
       <c r="Z16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AA16" s="11" t="s">
+      <c r="AB16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AB16" s="11" t="s">
+      <c r="AC16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AC16" s="11" t="s">
+      <c r="AD16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AD16" s="11" t="s">
+      <c r="AE16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AE16" s="11" t="s">
+      <c r="AF16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AF16" s="11" t="s">
+      <c r="AG16" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="AG16" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="AH16" s="11" t="s">
         <v>16</v>
@@ -2179,28 +2201,28 @@
         <v>18</v>
       </c>
       <c r="AK16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AL16" s="11" t="s">
+      <c r="AM16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AM16" s="11" t="s">
+      <c r="AN16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AN16" s="11" t="s">
+      <c r="AO16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AO16" s="11" t="s">
+      <c r="AP16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AP16" s="11" t="s">
+      <c r="AQ16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AQ16" s="11" t="s">
+      <c r="AR16" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="AR16" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="AS16" s="11" t="s">
         <v>16</v>
@@ -2212,28 +2234,28 @@
         <v>18</v>
       </c>
       <c r="AV16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="AW16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AW16" s="11" t="s">
+      <c r="AX16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AX16" s="11" t="s">
+      <c r="AY16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AY16" s="11" t="s">
+      <c r="AZ16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AZ16" s="11" t="s">
+      <c r="BA16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BA16" s="11" t="s">
+      <c r="BB16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="BB16" s="11" t="s">
+      <c r="BC16" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="BC16" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="BD16" s="11" t="s">
         <v>16</v>
@@ -2245,28 +2267,28 @@
         <v>18</v>
       </c>
       <c r="BG16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="BH16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BH16" s="11" t="s">
+      <c r="BI16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="BI16" s="11" t="s">
+      <c r="BJ16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="BJ16" s="11" t="s">
+      <c r="BK16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="BK16" s="11" t="s">
+      <c r="BL16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BL16" s="11" t="s">
+      <c r="BM16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="BM16" s="11" t="s">
+      <c r="BN16" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="BN16" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="BO16" s="11" t="s">
         <v>16</v>
@@ -2278,28 +2300,28 @@
         <v>18</v>
       </c>
       <c r="BR16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="BS16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BS16" s="11" t="s">
+      <c r="BT16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="BT16" s="11" t="s">
+      <c r="BU16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="BU16" s="11" t="s">
+      <c r="BV16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="BV16" s="11" t="s">
+      <c r="BW16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BW16" s="11" t="s">
+      <c r="BX16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="BX16" s="11" t="s">
+      <c r="BY16" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="BY16" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="BZ16" s="11" t="s">
         <v>16</v>
@@ -2311,28 +2333,28 @@
         <v>18</v>
       </c>
       <c r="CC16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="CD16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="CD16" s="11" t="s">
+      <c r="CE16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="CE16" s="11" t="s">
+      <c r="CF16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="CF16" s="11" t="s">
+      <c r="CG16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="CG16" s="11" t="s">
+      <c r="CH16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="CH16" s="11" t="s">
+      <c r="CI16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="CI16" s="11" t="s">
+      <c r="CJ16" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="CJ16" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="CK16" s="11" t="s">
         <v>16</v>
@@ -2344,28 +2366,28 @@
         <v>18</v>
       </c>
       <c r="CN16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="CO16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="CO16" s="11" t="s">
+      <c r="CP16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="CP16" s="11" t="s">
+      <c r="CQ16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="CQ16" s="11" t="s">
+      <c r="CR16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="CR16" s="11" t="s">
+      <c r="CS16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="CS16" s="11" t="s">
+      <c r="CT16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="CT16" s="11" t="s">
+      <c r="CU16" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="CU16" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="CV16" s="11" t="s">
         <v>16</v>
@@ -2377,28 +2399,28 @@
         <v>18</v>
       </c>
       <c r="CY16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="CZ16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="CZ16" s="11" t="s">
+      <c r="DA16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="DA16" s="11" t="s">
+      <c r="DB16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="DB16" s="11" t="s">
+      <c r="DC16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="DC16" s="11" t="s">
+      <c r="DD16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="DD16" s="11" t="s">
+      <c r="DE16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="DE16" s="11" t="s">
+      <c r="DF16" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="DF16" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="DG16" s="11" t="s">
         <v>16</v>
@@ -2410,37 +2432,37 @@
         <v>18</v>
       </c>
       <c r="DJ16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="DK16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="DK16" s="11" t="s">
+      <c r="DL16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="DL16" s="11" t="s">
+      <c r="DM16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="DM16" s="11" t="s">
+      <c r="DN16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="DN16" s="11" t="s">
+      <c r="DO16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="DO16" s="11" t="s">
+      <c r="DP16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="DP16" s="11" t="s">
+      <c r="DQ16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="DQ16" s="11" t="s">
+      <c r="DR16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="DR16" s="11" t="s">
+      <c r="DS16" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="DS16" s="11" t="s">
+      <c r="DT16" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="DT16" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="DU16" s="13" t="s">
         <v>19</v>
@@ -2449,6 +2471,67 @@
     </row>
   </sheetData>
   <mergeCells count="77">
+    <mergeCell ref="DG13:DQ13"/>
+    <mergeCell ref="DG14:DG15"/>
+    <mergeCell ref="DH14:DH15"/>
+    <mergeCell ref="DI14:DI15"/>
+    <mergeCell ref="DJ14:DJ15"/>
+    <mergeCell ref="DK14:DQ14"/>
+    <mergeCell ref="CV13:DF13"/>
+    <mergeCell ref="CV14:CV15"/>
+    <mergeCell ref="CW14:CW15"/>
+    <mergeCell ref="CX14:CX15"/>
+    <mergeCell ref="CY14:CY15"/>
+    <mergeCell ref="CZ14:DF14"/>
+    <mergeCell ref="CK13:CU13"/>
+    <mergeCell ref="CK14:CK15"/>
+    <mergeCell ref="CL14:CL15"/>
+    <mergeCell ref="CM14:CM15"/>
+    <mergeCell ref="CN14:CN15"/>
+    <mergeCell ref="CO14:CU14"/>
+    <mergeCell ref="BZ13:CJ13"/>
+    <mergeCell ref="BZ14:BZ15"/>
+    <mergeCell ref="CA14:CA15"/>
+    <mergeCell ref="CB14:CB15"/>
+    <mergeCell ref="CC14:CC15"/>
+    <mergeCell ref="CD14:CJ14"/>
+    <mergeCell ref="BO13:BY13"/>
+    <mergeCell ref="BO14:BO15"/>
+    <mergeCell ref="BP14:BP15"/>
+    <mergeCell ref="BQ14:BQ15"/>
+    <mergeCell ref="BR14:BR15"/>
+    <mergeCell ref="BS14:BY14"/>
+    <mergeCell ref="AS13:BC13"/>
+    <mergeCell ref="AS14:AS15"/>
+    <mergeCell ref="AT14:AT15"/>
+    <mergeCell ref="AU14:AU15"/>
+    <mergeCell ref="AV14:AV15"/>
+    <mergeCell ref="AW14:BC14"/>
+    <mergeCell ref="BH14:BN14"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="DS13:DS15"/>
+    <mergeCell ref="DT13:DT15"/>
+    <mergeCell ref="AJ14:AJ15"/>
+    <mergeCell ref="AK14:AK15"/>
+    <mergeCell ref="L13:V13"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="W14:W15"/>
+    <mergeCell ref="BD13:BN13"/>
+    <mergeCell ref="BD14:BD15"/>
+    <mergeCell ref="BE14:BE15"/>
+    <mergeCell ref="BF14:BF15"/>
+    <mergeCell ref="BG14:BG15"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="P14:V14"/>
@@ -2465,67 +2548,6 @@
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="K13:K15"/>
     <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="DS13:DS15"/>
-    <mergeCell ref="DT13:DT15"/>
-    <mergeCell ref="AJ14:AJ15"/>
-    <mergeCell ref="AK14:AK15"/>
-    <mergeCell ref="L13:V13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="W14:W15"/>
-    <mergeCell ref="BD13:BN13"/>
-    <mergeCell ref="BD14:BD15"/>
-    <mergeCell ref="BE14:BE15"/>
-    <mergeCell ref="BF14:BF15"/>
-    <mergeCell ref="BG14:BG15"/>
-    <mergeCell ref="BH14:BN14"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="AS13:BC13"/>
-    <mergeCell ref="AS14:AS15"/>
-    <mergeCell ref="AT14:AT15"/>
-    <mergeCell ref="AU14:AU15"/>
-    <mergeCell ref="AV14:AV15"/>
-    <mergeCell ref="AW14:BC14"/>
-    <mergeCell ref="BO13:BY13"/>
-    <mergeCell ref="BO14:BO15"/>
-    <mergeCell ref="BP14:BP15"/>
-    <mergeCell ref="BQ14:BQ15"/>
-    <mergeCell ref="BR14:BR15"/>
-    <mergeCell ref="BS14:BY14"/>
-    <mergeCell ref="BZ13:CJ13"/>
-    <mergeCell ref="BZ14:BZ15"/>
-    <mergeCell ref="CA14:CA15"/>
-    <mergeCell ref="CB14:CB15"/>
-    <mergeCell ref="CC14:CC15"/>
-    <mergeCell ref="CD14:CJ14"/>
-    <mergeCell ref="CK13:CU13"/>
-    <mergeCell ref="CK14:CK15"/>
-    <mergeCell ref="CL14:CL15"/>
-    <mergeCell ref="CM14:CM15"/>
-    <mergeCell ref="CN14:CN15"/>
-    <mergeCell ref="CO14:CU14"/>
-    <mergeCell ref="CV13:DF13"/>
-    <mergeCell ref="CV14:CV15"/>
-    <mergeCell ref="CW14:CW15"/>
-    <mergeCell ref="CX14:CX15"/>
-    <mergeCell ref="CY14:CY15"/>
-    <mergeCell ref="CZ14:DF14"/>
-    <mergeCell ref="DG13:DQ13"/>
-    <mergeCell ref="DG14:DG15"/>
-    <mergeCell ref="DH14:DH15"/>
-    <mergeCell ref="DI14:DI15"/>
-    <mergeCell ref="DJ14:DJ15"/>
-    <mergeCell ref="DK14:DQ14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
EBEGU-2013: Gesuche without angebot are not included in the statistic - The problem was that gesuche without angebot were marked as BG_GESUCH and not as NO_ANGEBOT_GESUCH - some refactoring
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Massenversand.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Massenversand.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denise\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16D46E4-9B09-41E7-93BD-7EEFCC6169C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD77B86-C7A9-45BB-8CF5-1B239ABF57B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10590" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,10 +460,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -483,8 +481,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,8 +897,8 @@
   </sheetPr>
   <dimension ref="A1:DV16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13:K15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,10 +1080,10 @@
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="20"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -1422,425 +1422,425 @@
       </c>
     </row>
     <row r="13" spans="1:126" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="21" t="s">
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="L13" s="28" t="s">
+      <c r="L13" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
-      <c r="W13" s="28" t="s">
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="28"/>
-      <c r="Z13" s="28"/>
-      <c r="AA13" s="28"/>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="28"/>
-      <c r="AD13" s="28"/>
-      <c r="AE13" s="28"/>
-      <c r="AF13" s="28"/>
-      <c r="AG13" s="28"/>
-      <c r="AH13" s="28" t="s">
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="19"/>
+      <c r="AG13" s="19"/>
+      <c r="AH13" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="AI13" s="28"/>
-      <c r="AJ13" s="28"/>
-      <c r="AK13" s="28"/>
-      <c r="AL13" s="28"/>
-      <c r="AM13" s="28"/>
-      <c r="AN13" s="28"/>
-      <c r="AO13" s="28"/>
-      <c r="AP13" s="28"/>
-      <c r="AQ13" s="28"/>
-      <c r="AR13" s="28"/>
-      <c r="AS13" s="28" t="s">
+      <c r="AI13" s="19"/>
+      <c r="AJ13" s="19"/>
+      <c r="AK13" s="19"/>
+      <c r="AL13" s="19"/>
+      <c r="AM13" s="19"/>
+      <c r="AN13" s="19"/>
+      <c r="AO13" s="19"/>
+      <c r="AP13" s="19"/>
+      <c r="AQ13" s="19"/>
+      <c r="AR13" s="19"/>
+      <c r="AS13" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="AT13" s="28"/>
-      <c r="AU13" s="28"/>
-      <c r="AV13" s="28"/>
-      <c r="AW13" s="28"/>
-      <c r="AX13" s="28"/>
-      <c r="AY13" s="28"/>
-      <c r="AZ13" s="28"/>
-      <c r="BA13" s="28"/>
-      <c r="BB13" s="28"/>
-      <c r="BC13" s="28"/>
-      <c r="BD13" s="28" t="s">
+      <c r="AT13" s="19"/>
+      <c r="AU13" s="19"/>
+      <c r="AV13" s="19"/>
+      <c r="AW13" s="19"/>
+      <c r="AX13" s="19"/>
+      <c r="AY13" s="19"/>
+      <c r="AZ13" s="19"/>
+      <c r="BA13" s="19"/>
+      <c r="BB13" s="19"/>
+      <c r="BC13" s="19"/>
+      <c r="BD13" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="BE13" s="28"/>
-      <c r="BF13" s="28"/>
-      <c r="BG13" s="28"/>
-      <c r="BH13" s="28"/>
-      <c r="BI13" s="28"/>
-      <c r="BJ13" s="28"/>
-      <c r="BK13" s="28"/>
-      <c r="BL13" s="28"/>
-      <c r="BM13" s="28"/>
-      <c r="BN13" s="28"/>
-      <c r="BO13" s="28" t="s">
+      <c r="BE13" s="19"/>
+      <c r="BF13" s="19"/>
+      <c r="BG13" s="19"/>
+      <c r="BH13" s="19"/>
+      <c r="BI13" s="19"/>
+      <c r="BJ13" s="19"/>
+      <c r="BK13" s="19"/>
+      <c r="BL13" s="19"/>
+      <c r="BM13" s="19"/>
+      <c r="BN13" s="19"/>
+      <c r="BO13" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="BP13" s="28"/>
-      <c r="BQ13" s="28"/>
-      <c r="BR13" s="28"/>
-      <c r="BS13" s="28"/>
-      <c r="BT13" s="28"/>
-      <c r="BU13" s="28"/>
-      <c r="BV13" s="28"/>
-      <c r="BW13" s="28"/>
-      <c r="BX13" s="28"/>
-      <c r="BY13" s="28"/>
-      <c r="BZ13" s="28" t="s">
+      <c r="BP13" s="19"/>
+      <c r="BQ13" s="19"/>
+      <c r="BR13" s="19"/>
+      <c r="BS13" s="19"/>
+      <c r="BT13" s="19"/>
+      <c r="BU13" s="19"/>
+      <c r="BV13" s="19"/>
+      <c r="BW13" s="19"/>
+      <c r="BX13" s="19"/>
+      <c r="BY13" s="19"/>
+      <c r="BZ13" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="CA13" s="28"/>
-      <c r="CB13" s="28"/>
-      <c r="CC13" s="28"/>
-      <c r="CD13" s="28"/>
-      <c r="CE13" s="28"/>
-      <c r="CF13" s="28"/>
-      <c r="CG13" s="28"/>
-      <c r="CH13" s="28"/>
-      <c r="CI13" s="28"/>
-      <c r="CJ13" s="28"/>
-      <c r="CK13" s="28" t="s">
+      <c r="CA13" s="19"/>
+      <c r="CB13" s="19"/>
+      <c r="CC13" s="19"/>
+      <c r="CD13" s="19"/>
+      <c r="CE13" s="19"/>
+      <c r="CF13" s="19"/>
+      <c r="CG13" s="19"/>
+      <c r="CH13" s="19"/>
+      <c r="CI13" s="19"/>
+      <c r="CJ13" s="19"/>
+      <c r="CK13" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="CL13" s="28"/>
-      <c r="CM13" s="28"/>
-      <c r="CN13" s="28"/>
-      <c r="CO13" s="28"/>
-      <c r="CP13" s="28"/>
-      <c r="CQ13" s="28"/>
-      <c r="CR13" s="28"/>
-      <c r="CS13" s="28"/>
-      <c r="CT13" s="28"/>
-      <c r="CU13" s="28"/>
-      <c r="CV13" s="28" t="s">
+      <c r="CL13" s="19"/>
+      <c r="CM13" s="19"/>
+      <c r="CN13" s="19"/>
+      <c r="CO13" s="19"/>
+      <c r="CP13" s="19"/>
+      <c r="CQ13" s="19"/>
+      <c r="CR13" s="19"/>
+      <c r="CS13" s="19"/>
+      <c r="CT13" s="19"/>
+      <c r="CU13" s="19"/>
+      <c r="CV13" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="CW13" s="28"/>
-      <c r="CX13" s="28"/>
-      <c r="CY13" s="28"/>
-      <c r="CZ13" s="28"/>
-      <c r="DA13" s="28"/>
-      <c r="DB13" s="28"/>
-      <c r="DC13" s="28"/>
-      <c r="DD13" s="28"/>
-      <c r="DE13" s="28"/>
-      <c r="DF13" s="28"/>
-      <c r="DG13" s="28" t="s">
+      <c r="CW13" s="19"/>
+      <c r="CX13" s="19"/>
+      <c r="CY13" s="19"/>
+      <c r="CZ13" s="19"/>
+      <c r="DA13" s="19"/>
+      <c r="DB13" s="19"/>
+      <c r="DC13" s="19"/>
+      <c r="DD13" s="19"/>
+      <c r="DE13" s="19"/>
+      <c r="DF13" s="19"/>
+      <c r="DG13" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="DH13" s="28"/>
-      <c r="DI13" s="28"/>
-      <c r="DJ13" s="28"/>
-      <c r="DK13" s="28"/>
-      <c r="DL13" s="28"/>
-      <c r="DM13" s="28"/>
-      <c r="DN13" s="28"/>
-      <c r="DO13" s="28"/>
-      <c r="DP13" s="28"/>
-      <c r="DQ13" s="28"/>
-      <c r="DR13" s="25" t="s">
+      <c r="DH13" s="19"/>
+      <c r="DI13" s="19"/>
+      <c r="DJ13" s="19"/>
+      <c r="DK13" s="19"/>
+      <c r="DL13" s="19"/>
+      <c r="DM13" s="19"/>
+      <c r="DN13" s="19"/>
+      <c r="DO13" s="19"/>
+      <c r="DP13" s="19"/>
+      <c r="DQ13" s="19"/>
+      <c r="DR13" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="DS13" s="25" t="s">
+      <c r="DS13" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="DT13" s="25" t="s">
+      <c r="DT13" s="23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:126" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="28" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="21"/>
-      <c r="L14" s="28" t="s">
+      <c r="K14" s="28"/>
+      <c r="L14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="M14" s="28" t="s">
+      <c r="M14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="N14" s="28" t="s">
+      <c r="N14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="28" t="s">
+      <c r="O14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="P14" s="22" t="s">
+      <c r="P14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="28" t="s">
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="X14" s="28" t="s">
+      <c r="X14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="Y14" s="28" t="s">
+      <c r="Y14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="Z14" s="28" t="s">
+      <c r="Z14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="AA14" s="22" t="s">
+      <c r="AA14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="AB14" s="23"/>
-      <c r="AC14" s="23"/>
-      <c r="AD14" s="23"/>
-      <c r="AE14" s="23"/>
-      <c r="AF14" s="23"/>
-      <c r="AG14" s="24"/>
-      <c r="AH14" s="28" t="s">
+      <c r="AB14" s="21"/>
+      <c r="AC14" s="21"/>
+      <c r="AD14" s="21"/>
+      <c r="AE14" s="21"/>
+      <c r="AF14" s="21"/>
+      <c r="AG14" s="22"/>
+      <c r="AH14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AI14" s="28" t="s">
+      <c r="AI14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AJ14" s="28" t="s">
+      <c r="AJ14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AK14" s="28" t="s">
+      <c r="AK14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="AL14" s="22" t="s">
+      <c r="AL14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="AM14" s="23"/>
-      <c r="AN14" s="23"/>
-      <c r="AO14" s="23"/>
-      <c r="AP14" s="23"/>
-      <c r="AQ14" s="23"/>
-      <c r="AR14" s="24"/>
-      <c r="AS14" s="28" t="s">
+      <c r="AM14" s="21"/>
+      <c r="AN14" s="21"/>
+      <c r="AO14" s="21"/>
+      <c r="AP14" s="21"/>
+      <c r="AQ14" s="21"/>
+      <c r="AR14" s="22"/>
+      <c r="AS14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AT14" s="28" t="s">
+      <c r="AT14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AU14" s="28" t="s">
+      <c r="AU14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AV14" s="28" t="s">
+      <c r="AV14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="AW14" s="22" t="s">
+      <c r="AW14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="AX14" s="23"/>
-      <c r="AY14" s="23"/>
-      <c r="AZ14" s="23"/>
-      <c r="BA14" s="23"/>
-      <c r="BB14" s="23"/>
-      <c r="BC14" s="24"/>
-      <c r="BD14" s="28" t="s">
+      <c r="AX14" s="21"/>
+      <c r="AY14" s="21"/>
+      <c r="AZ14" s="21"/>
+      <c r="BA14" s="21"/>
+      <c r="BB14" s="21"/>
+      <c r="BC14" s="22"/>
+      <c r="BD14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="BE14" s="28" t="s">
+      <c r="BE14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="BF14" s="28" t="s">
+      <c r="BF14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="BG14" s="28" t="s">
+      <c r="BG14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="BH14" s="22" t="s">
+      <c r="BH14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="BI14" s="23"/>
-      <c r="BJ14" s="23"/>
-      <c r="BK14" s="23"/>
-      <c r="BL14" s="23"/>
-      <c r="BM14" s="23"/>
-      <c r="BN14" s="24"/>
-      <c r="BO14" s="28" t="s">
+      <c r="BI14" s="21"/>
+      <c r="BJ14" s="21"/>
+      <c r="BK14" s="21"/>
+      <c r="BL14" s="21"/>
+      <c r="BM14" s="21"/>
+      <c r="BN14" s="22"/>
+      <c r="BO14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="BP14" s="28" t="s">
+      <c r="BP14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="BQ14" s="28" t="s">
+      <c r="BQ14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="BR14" s="28" t="s">
+      <c r="BR14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="BS14" s="22" t="s">
+      <c r="BS14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="BT14" s="23"/>
-      <c r="BU14" s="23"/>
-      <c r="BV14" s="23"/>
-      <c r="BW14" s="23"/>
-      <c r="BX14" s="23"/>
-      <c r="BY14" s="24"/>
-      <c r="BZ14" s="28" t="s">
+      <c r="BT14" s="21"/>
+      <c r="BU14" s="21"/>
+      <c r="BV14" s="21"/>
+      <c r="BW14" s="21"/>
+      <c r="BX14" s="21"/>
+      <c r="BY14" s="22"/>
+      <c r="BZ14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="CA14" s="28" t="s">
+      <c r="CA14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CB14" s="28" t="s">
+      <c r="CB14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="CC14" s="28" t="s">
+      <c r="CC14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="CD14" s="22" t="s">
+      <c r="CD14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="CE14" s="23"/>
-      <c r="CF14" s="23"/>
-      <c r="CG14" s="23"/>
-      <c r="CH14" s="23"/>
-      <c r="CI14" s="23"/>
-      <c r="CJ14" s="24"/>
-      <c r="CK14" s="28" t="s">
+      <c r="CE14" s="21"/>
+      <c r="CF14" s="21"/>
+      <c r="CG14" s="21"/>
+      <c r="CH14" s="21"/>
+      <c r="CI14" s="21"/>
+      <c r="CJ14" s="22"/>
+      <c r="CK14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="CL14" s="28" t="s">
+      <c r="CL14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CM14" s="28" t="s">
+      <c r="CM14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="CN14" s="28" t="s">
+      <c r="CN14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="CO14" s="22" t="s">
+      <c r="CO14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="CP14" s="23"/>
-      <c r="CQ14" s="23"/>
-      <c r="CR14" s="23"/>
-      <c r="CS14" s="23"/>
-      <c r="CT14" s="23"/>
-      <c r="CU14" s="24"/>
-      <c r="CV14" s="28" t="s">
+      <c r="CP14" s="21"/>
+      <c r="CQ14" s="21"/>
+      <c r="CR14" s="21"/>
+      <c r="CS14" s="21"/>
+      <c r="CT14" s="21"/>
+      <c r="CU14" s="22"/>
+      <c r="CV14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="CW14" s="28" t="s">
+      <c r="CW14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="CX14" s="28" t="s">
+      <c r="CX14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="CY14" s="28" t="s">
+      <c r="CY14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="CZ14" s="22" t="s">
+      <c r="CZ14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="DA14" s="23"/>
-      <c r="DB14" s="23"/>
-      <c r="DC14" s="23"/>
-      <c r="DD14" s="23"/>
-      <c r="DE14" s="23"/>
-      <c r="DF14" s="24"/>
-      <c r="DG14" s="28" t="s">
+      <c r="DA14" s="21"/>
+      <c r="DB14" s="21"/>
+      <c r="DC14" s="21"/>
+      <c r="DD14" s="21"/>
+      <c r="DE14" s="21"/>
+      <c r="DF14" s="22"/>
+      <c r="DG14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="DH14" s="28" t="s">
+      <c r="DH14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="DI14" s="28" t="s">
+      <c r="DI14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="DJ14" s="28" t="s">
+      <c r="DJ14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="DK14" s="22" t="s">
+      <c r="DK14" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="DL14" s="23"/>
-      <c r="DM14" s="23"/>
-      <c r="DN14" s="23"/>
-      <c r="DO14" s="23"/>
-      <c r="DP14" s="23"/>
-      <c r="DQ14" s="24"/>
-      <c r="DR14" s="26"/>
-      <c r="DS14" s="26"/>
-      <c r="DT14" s="26"/>
+      <c r="DL14" s="21"/>
+      <c r="DM14" s="21"/>
+      <c r="DN14" s="21"/>
+      <c r="DO14" s="21"/>
+      <c r="DP14" s="21"/>
+      <c r="DQ14" s="22"/>
+      <c r="DR14" s="24"/>
+      <c r="DS14" s="24"/>
+      <c r="DT14" s="24"/>
     </row>
     <row r="15" spans="1:126" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
       <c r="P15" s="12" t="s">
         <v>43</v>
       </c>
@@ -1862,10 +1862,10 @@
       <c r="V15" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="W15" s="28"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="28"/>
-      <c r="Z15" s="28"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
       <c r="AA15" s="12" t="s">
         <v>43</v>
       </c>
@@ -1887,10 +1887,10 @@
       <c r="AG15" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AH15" s="28"/>
-      <c r="AI15" s="28"/>
-      <c r="AJ15" s="28"/>
-      <c r="AK15" s="28"/>
+      <c r="AH15" s="19"/>
+      <c r="AI15" s="19"/>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="19"/>
       <c r="AL15" s="12" t="s">
         <v>43</v>
       </c>
@@ -1912,10 +1912,10 @@
       <c r="AR15" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AS15" s="28"/>
-      <c r="AT15" s="28"/>
-      <c r="AU15" s="28"/>
-      <c r="AV15" s="28"/>
+      <c r="AS15" s="19"/>
+      <c r="AT15" s="19"/>
+      <c r="AU15" s="19"/>
+      <c r="AV15" s="19"/>
       <c r="AW15" s="14" t="s">
         <v>43</v>
       </c>
@@ -1937,10 +1937,10 @@
       <c r="BC15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="BD15" s="28"/>
-      <c r="BE15" s="28"/>
-      <c r="BF15" s="28"/>
-      <c r="BG15" s="28"/>
+      <c r="BD15" s="19"/>
+      <c r="BE15" s="19"/>
+      <c r="BF15" s="19"/>
+      <c r="BG15" s="19"/>
       <c r="BH15" s="14" t="s">
         <v>43</v>
       </c>
@@ -1962,10 +1962,10 @@
       <c r="BN15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="BO15" s="28"/>
-      <c r="BP15" s="28"/>
-      <c r="BQ15" s="28"/>
-      <c r="BR15" s="28"/>
+      <c r="BO15" s="19"/>
+      <c r="BP15" s="19"/>
+      <c r="BQ15" s="19"/>
+      <c r="BR15" s="19"/>
       <c r="BS15" s="14" t="s">
         <v>43</v>
       </c>
@@ -1987,10 +1987,10 @@
       <c r="BY15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="BZ15" s="28"/>
-      <c r="CA15" s="28"/>
-      <c r="CB15" s="28"/>
-      <c r="CC15" s="28"/>
+      <c r="BZ15" s="19"/>
+      <c r="CA15" s="19"/>
+      <c r="CB15" s="19"/>
+      <c r="CC15" s="19"/>
       <c r="CD15" s="14" t="s">
         <v>43</v>
       </c>
@@ -2012,10 +2012,10 @@
       <c r="CJ15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="CK15" s="28"/>
-      <c r="CL15" s="28"/>
-      <c r="CM15" s="28"/>
-      <c r="CN15" s="28"/>
+      <c r="CK15" s="19"/>
+      <c r="CL15" s="19"/>
+      <c r="CM15" s="19"/>
+      <c r="CN15" s="19"/>
       <c r="CO15" s="14" t="s">
         <v>43</v>
       </c>
@@ -2037,10 +2037,10 @@
       <c r="CU15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="CV15" s="28"/>
-      <c r="CW15" s="28"/>
-      <c r="CX15" s="28"/>
-      <c r="CY15" s="28"/>
+      <c r="CV15" s="19"/>
+      <c r="CW15" s="19"/>
+      <c r="CX15" s="19"/>
+      <c r="CY15" s="19"/>
       <c r="CZ15" s="14" t="s">
         <v>43</v>
       </c>
@@ -2062,10 +2062,10 @@
       <c r="DF15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="DG15" s="28"/>
-      <c r="DH15" s="28"/>
-      <c r="DI15" s="28"/>
-      <c r="DJ15" s="28"/>
+      <c r="DG15" s="19"/>
+      <c r="DH15" s="19"/>
+      <c r="DI15" s="19"/>
+      <c r="DJ15" s="19"/>
       <c r="DK15" s="14" t="s">
         <v>43</v>
       </c>
@@ -2087,9 +2087,9 @@
       <c r="DQ15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="DR15" s="27"/>
-      <c r="DS15" s="27"/>
-      <c r="DT15" s="27"/>
+      <c r="DR15" s="25"/>
+      <c r="DS15" s="25"/>
+      <c r="DT15" s="25"/>
     </row>
     <row r="16" spans="1:126" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
@@ -2471,51 +2471,22 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="DG13:DQ13"/>
-    <mergeCell ref="DG14:DG15"/>
-    <mergeCell ref="DH14:DH15"/>
-    <mergeCell ref="DI14:DI15"/>
-    <mergeCell ref="DJ14:DJ15"/>
-    <mergeCell ref="DK14:DQ14"/>
-    <mergeCell ref="CV13:DF13"/>
-    <mergeCell ref="CV14:CV15"/>
-    <mergeCell ref="CW14:CW15"/>
-    <mergeCell ref="CX14:CX15"/>
-    <mergeCell ref="CY14:CY15"/>
-    <mergeCell ref="CZ14:DF14"/>
-    <mergeCell ref="CK13:CU13"/>
-    <mergeCell ref="CK14:CK15"/>
-    <mergeCell ref="CL14:CL15"/>
-    <mergeCell ref="CM14:CM15"/>
-    <mergeCell ref="CN14:CN15"/>
-    <mergeCell ref="CO14:CU14"/>
-    <mergeCell ref="BZ13:CJ13"/>
-    <mergeCell ref="BZ14:BZ15"/>
-    <mergeCell ref="CA14:CA15"/>
-    <mergeCell ref="CB14:CB15"/>
-    <mergeCell ref="CC14:CC15"/>
-    <mergeCell ref="CD14:CJ14"/>
-    <mergeCell ref="BO13:BY13"/>
-    <mergeCell ref="BO14:BO15"/>
-    <mergeCell ref="BP14:BP15"/>
-    <mergeCell ref="BQ14:BQ15"/>
-    <mergeCell ref="BR14:BR15"/>
-    <mergeCell ref="BS14:BY14"/>
-    <mergeCell ref="AS13:BC13"/>
-    <mergeCell ref="AS14:AS15"/>
-    <mergeCell ref="AT14:AT15"/>
-    <mergeCell ref="AU14:AU15"/>
-    <mergeCell ref="AV14:AV15"/>
-    <mergeCell ref="AW14:BC14"/>
-    <mergeCell ref="BH14:BN14"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="P14:V14"/>
+    <mergeCell ref="DR13:DR15"/>
+    <mergeCell ref="W13:AG13"/>
+    <mergeCell ref="AA14:AG14"/>
+    <mergeCell ref="AH13:AR13"/>
+    <mergeCell ref="AH14:AH15"/>
+    <mergeCell ref="AI14:AI15"/>
+    <mergeCell ref="AL14:AR14"/>
+    <mergeCell ref="Z14:Z15"/>
+    <mergeCell ref="Y14:Y15"/>
+    <mergeCell ref="X14:X15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="C13:F13"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="DS13:DS15"/>
     <mergeCell ref="DT13:DT15"/>
@@ -2532,22 +2503,51 @@
     <mergeCell ref="BE14:BE15"/>
     <mergeCell ref="BF14:BF15"/>
     <mergeCell ref="BG14:BG15"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="P14:V14"/>
-    <mergeCell ref="DR13:DR15"/>
-    <mergeCell ref="W13:AG13"/>
-    <mergeCell ref="AA14:AG14"/>
-    <mergeCell ref="AH13:AR13"/>
-    <mergeCell ref="AH14:AH15"/>
-    <mergeCell ref="AI14:AI15"/>
-    <mergeCell ref="AL14:AR14"/>
-    <mergeCell ref="Z14:Z15"/>
-    <mergeCell ref="Y14:Y15"/>
-    <mergeCell ref="X14:X15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="BH14:BN14"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="AS13:BC13"/>
+    <mergeCell ref="AS14:AS15"/>
+    <mergeCell ref="AT14:AT15"/>
+    <mergeCell ref="AU14:AU15"/>
+    <mergeCell ref="AV14:AV15"/>
+    <mergeCell ref="AW14:BC14"/>
+    <mergeCell ref="BO13:BY13"/>
+    <mergeCell ref="BO14:BO15"/>
+    <mergeCell ref="BP14:BP15"/>
+    <mergeCell ref="BQ14:BQ15"/>
+    <mergeCell ref="BR14:BR15"/>
+    <mergeCell ref="BS14:BY14"/>
+    <mergeCell ref="BZ13:CJ13"/>
+    <mergeCell ref="BZ14:BZ15"/>
+    <mergeCell ref="CA14:CA15"/>
+    <mergeCell ref="CB14:CB15"/>
+    <mergeCell ref="CC14:CC15"/>
+    <mergeCell ref="CD14:CJ14"/>
+    <mergeCell ref="CK13:CU13"/>
+    <mergeCell ref="CK14:CK15"/>
+    <mergeCell ref="CL14:CL15"/>
+    <mergeCell ref="CM14:CM15"/>
+    <mergeCell ref="CN14:CN15"/>
+    <mergeCell ref="CO14:CU14"/>
+    <mergeCell ref="CV13:DF13"/>
+    <mergeCell ref="CV14:CV15"/>
+    <mergeCell ref="CW14:CW15"/>
+    <mergeCell ref="CX14:CX15"/>
+    <mergeCell ref="CY14:CY15"/>
+    <mergeCell ref="CZ14:DF14"/>
+    <mergeCell ref="DG13:DQ13"/>
+    <mergeCell ref="DG14:DG15"/>
+    <mergeCell ref="DH14:DH15"/>
+    <mergeCell ref="DI14:DI15"/>
+    <mergeCell ref="DJ14:DJ15"/>
+    <mergeCell ref="DK14:DQ14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>